<commit_message>
Minor updates to the guidelines
</commit_message>
<xml_diff>
--- a/scripts and their roles.xlsx
+++ b/scripts and their roles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\sync\Green Pheasants\Data and code\Production\Green-Pheasants-Public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD39727-9648-4B3D-A0E6-CDF9FBE2B625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605418D3-CE08-4ECF-A31B-0F4645FBC02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,15 +56,9 @@
     <t>All of the functions</t>
   </si>
   <si>
-    <t>training_visitors</t>
-  </si>
-  <si>
     <t>Trains the model that chooses items for visitors</t>
   </si>
   <si>
-    <t>training_users</t>
-  </si>
-  <si>
     <t>Trains the model that chooses items for users</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
     <t>Script</t>
   </si>
   <si>
-    <t>When we send users items  via email or app</t>
-  </si>
-  <si>
     <t>df_items_with_betas</t>
   </si>
   <si>
@@ -119,13 +110,22 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Every six hours</t>
-  </si>
-  <si>
     <t>Run once, and then re-run only when one of the functions is changed</t>
   </si>
   <si>
     <t>The information in df_results should automatically be added to the row that describes the interaction in the interactions dataframe</t>
+  </si>
+  <si>
+    <t>Every 24 hours, at GMT-10</t>
+  </si>
+  <si>
+    <t>Right after running the train_users script at GMT-10</t>
+  </si>
+  <si>
+    <t>train_visitors</t>
+  </si>
+  <si>
+    <t>train_users</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,12 +482,12 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -513,13 +513,13 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -528,19 +528,19 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -549,19 +549,19 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
         <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -570,19 +570,19 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -591,19 +591,19 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -612,24 +612,24 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>